<commit_message>
handling login functionality using excelsheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/jala/qa/testdata/Excel.xlsx
+++ b/src/main/java/com/jala/qa/testdata/Excel.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17424" windowHeight="3228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17424" windowHeight="3036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ali" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J7"/>
+  <oleSize ref="A1:Q8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Admin</t>
   </si>
@@ -72,13 +72,37 @@
   </si>
   <si>
     <t>Admin123</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>fks</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>fcsdc</t>
+  </si>
+  <si>
+    <t>training@jalaacademy.com</t>
+  </si>
+  <si>
+    <t>jobprogram</t>
+  </si>
+  <si>
+    <t>fghgh</t>
+  </si>
+  <si>
+    <t>dfggd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +129,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -166,6 +196,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,13 +601,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -592,7 +629,40 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>